<commit_message>
Added residuals analysis and plots. Fixed a typo in KOH data.
</commit_message>
<xml_diff>
--- a/data/KOH_data.xlsx
+++ b/data/KOH_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahbritton/Documents/Dissertation/Ch4_DietTradeOffs/tradeoff_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B402760-AFC8-D643-A469-B7C69DF58403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81C09E8-6FB7-D741-B006-E0512613906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="500" windowWidth="27640" windowHeight="16060" activeTab="1" xr2:uid="{F3F8205F-0BC4-1940-892C-1E5A2C216DA4}"/>
   </bookViews>
@@ -420,9 +420,6 @@
     <t>T365</t>
   </si>
   <si>
-    <t>T3456</t>
-  </si>
-  <si>
     <t>Thorax in 2 pieces- but seems ok!</t>
   </si>
   <si>
@@ -496,6 +493,9 @@
   </si>
   <si>
     <t>exclude</t>
+  </si>
+  <si>
+    <t>T346</t>
   </si>
 </sst>
 </file>
@@ -5773,16 +5773,16 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -6065,7 +6065,7 @@
   <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6083,25 +6083,25 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -6121,11 +6121,11 @@
         <v>1.5900000000000001E-2</v>
       </c>
       <c r="F2" s="2">
-        <f>D2-E2</f>
+        <f t="shared" ref="F2:F33" si="0">D2-E2</f>
         <v>6.8699999999999997E-2</v>
       </c>
       <c r="G2" s="2">
-        <f>F2/C2</f>
+        <f t="shared" ref="G2:G33" si="1">F2/C2</f>
         <v>9.6801465407918841E-2</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -6152,11 +6152,11 @@
         <v>1.84E-2</v>
       </c>
       <c r="F3" s="2">
-        <f>D3-E3</f>
+        <f t="shared" si="0"/>
         <v>7.7299999999999994E-2</v>
       </c>
       <c r="G3" s="2">
-        <f>F3/C3</f>
+        <f t="shared" si="1"/>
         <v>0.10412176724137931</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -6183,11 +6183,11 @@
         <v>1.83E-2</v>
       </c>
       <c r="F4" s="2">
-        <f>D4-E4</f>
+        <f t="shared" si="0"/>
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="G4" s="2">
-        <f>F4/C4</f>
+        <f t="shared" si="1"/>
         <v>9.9770796818120525E-2</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -6214,11 +6214,11 @@
         <v>1.3899999999999999E-2</v>
       </c>
       <c r="F5" s="2">
-        <f>D5-E5</f>
+        <f t="shared" si="0"/>
         <v>7.8399999999999997E-2</v>
       </c>
       <c r="G5" s="2">
-        <f>F5/C5</f>
+        <f t="shared" si="1"/>
         <v>0.15420928402832415</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -6245,11 +6245,11 @@
         <v>1.4200000000000001E-2</v>
       </c>
       <c r="F6" s="2">
-        <f>D6-E6</f>
+        <f t="shared" si="0"/>
         <v>5.7899999999999993E-2</v>
       </c>
       <c r="G6" s="2">
-        <f>F6/C6</f>
+        <f t="shared" si="1"/>
         <v>0.12277353689567429</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -6276,11 +6276,11 @@
         <v>1.9800000000000002E-2</v>
       </c>
       <c r="F7" s="2">
-        <f>D7-E7</f>
+        <f t="shared" si="0"/>
         <v>7.6399999999999996E-2</v>
       </c>
       <c r="G7" s="2">
-        <f>F7/C7</f>
+        <f t="shared" si="1"/>
         <v>0.10701778960638744</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -6307,11 +6307,11 @@
         <v>1.5299999999999999E-2</v>
       </c>
       <c r="F8" s="2">
-        <f>D8-E8</f>
+        <f t="shared" si="0"/>
         <v>7.0400000000000004E-2</v>
       </c>
       <c r="G8" s="2">
-        <f>F8/C8</f>
+        <f t="shared" si="1"/>
         <v>0.16356877323420074</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -6338,11 +6338,11 @@
         <v>1.38E-2</v>
       </c>
       <c r="F9" s="2">
-        <f>D9-E9</f>
+        <f t="shared" si="0"/>
         <v>6.3E-2</v>
       </c>
       <c r="G9" s="2">
-        <f>F9/C9</f>
+        <f t="shared" si="1"/>
         <v>0.13981358189081225</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -6369,11 +6369,11 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="F10" s="2">
-        <f>D10-E10</f>
+        <f t="shared" si="0"/>
         <v>8.4999999999999992E-2</v>
       </c>
       <c r="G10" s="2">
-        <f>F10/C10</f>
+        <f t="shared" si="1"/>
         <v>9.8243180767452601E-2</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -6397,11 +6397,11 @@
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="F11" s="2">
-        <f>D11-E11</f>
+        <f t="shared" si="0"/>
         <v>8.5300000000000001E-2</v>
       </c>
       <c r="G11" s="2">
-        <f>F11/C11</f>
+        <f t="shared" si="1"/>
         <v>0.15872720506140678</v>
       </c>
     </row>
@@ -6422,11 +6422,11 @@
         <v>1.15E-2</v>
       </c>
       <c r="F12" s="2">
-        <f>D12-E12</f>
+        <f t="shared" si="0"/>
         <v>6.9800000000000001E-2</v>
       </c>
       <c r="G12" s="2">
-        <f>F12/C12</f>
+        <f t="shared" si="1"/>
         <v>0.15388007054673722</v>
       </c>
     </row>
@@ -6447,11 +6447,11 @@
         <v>1.6299999999999999E-2</v>
       </c>
       <c r="F13" s="2">
-        <f>D13-E13</f>
+        <f t="shared" si="0"/>
         <v>8.7000000000000008E-2</v>
       </c>
       <c r="G13" s="2">
-        <f>F13/C13</f>
+        <f t="shared" si="1"/>
         <v>0.14121084239571499</v>
       </c>
       <c r="H13" s="3" t="s">
@@ -6475,11 +6475,11 @@
         <v>1.9699999999999999E-2</v>
       </c>
       <c r="F14" s="2">
-        <f>D14-E14</f>
+        <f t="shared" si="0"/>
         <v>9.2100000000000001E-2</v>
       </c>
       <c r="G14" s="2">
-        <f>F14/C14</f>
+        <f t="shared" si="1"/>
         <v>0.12289831865492395</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -6503,11 +6503,11 @@
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="F15" s="2">
-        <f>D15-E15</f>
+        <f t="shared" si="0"/>
         <v>7.7799999999999994E-2</v>
       </c>
       <c r="G15" s="2">
-        <f>F15/C15</f>
+        <f t="shared" si="1"/>
         <v>0.12706189776253471</v>
       </c>
     </row>
@@ -6528,11 +6528,11 @@
         <v>1.29E-2</v>
       </c>
       <c r="F16" s="2">
-        <f>D16-E16</f>
+        <f t="shared" si="0"/>
         <v>6.5300000000000011E-2</v>
       </c>
       <c r="G16" s="2">
-        <f>F16/C16</f>
+        <f t="shared" si="1"/>
         <v>0.13010559872484562</v>
       </c>
       <c r="H16" s="3" t="s">
@@ -6541,7 +6541,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="2">
         <v>6</v>
@@ -6556,11 +6556,11 @@
         <v>1.6299999999999999E-2</v>
       </c>
       <c r="F17" s="2">
-        <f>D17-E17</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="G17" s="2">
-        <f>F17/C17</f>
+        <f t="shared" si="1"/>
         <v>0.12152144853566656</v>
       </c>
     </row>
@@ -6581,11 +6581,11 @@
         <v>1.7299999999999999E-2</v>
       </c>
       <c r="F18" s="2">
-        <f>D18-E18</f>
+        <f t="shared" si="0"/>
         <v>0.1178</v>
       </c>
       <c r="G18" s="2">
-        <f>F18/C18</f>
+        <f t="shared" si="1"/>
         <v>0.17561121049493145</v>
       </c>
       <c r="H18" s="3" t="s">
@@ -6612,11 +6612,11 @@
         <v>1.9699999999999999E-2</v>
       </c>
       <c r="F19" s="2">
-        <f>D19-E19</f>
+        <f t="shared" si="0"/>
         <v>0.11200000000000002</v>
       </c>
       <c r="G19" s="2">
-        <f>F19/C19</f>
+        <f t="shared" si="1"/>
         <v>0.12839619396996449</v>
       </c>
     </row>
@@ -6637,11 +6637,11 @@
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="F20" s="2">
-        <f>D20-E20</f>
+        <f t="shared" si="0"/>
         <v>5.2499999999999998E-2</v>
       </c>
       <c r="G20" s="2">
-        <f>F20/C20</f>
+        <f t="shared" si="1"/>
         <v>0.10332611690612084</v>
       </c>
       <c r="H20" s="3" t="s">
@@ -6650,7 +6650,7 @@
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B21" s="2">
         <v>6</v>
@@ -6665,11 +6665,11 @@
         <v>1.15E-2</v>
       </c>
       <c r="F21" s="2">
-        <f>D21-E21</f>
+        <f t="shared" si="0"/>
         <v>8.7500000000000008E-2</v>
       </c>
       <c r="G21" s="2">
-        <f>F21/C21</f>
+        <f t="shared" si="1"/>
         <v>0.14800405953991883</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -6678,7 +6678,7 @@
     </row>
     <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B22" s="2">
         <v>6</v>
@@ -6693,11 +6693,11 @@
         <v>1.12E-2</v>
       </c>
       <c r="F22" s="2">
-        <f>D22-E22</f>
+        <f t="shared" si="0"/>
         <v>7.2599999999999998E-2</v>
       </c>
       <c r="G22" s="2">
-        <f>F22/C22</f>
+        <f t="shared" si="1"/>
         <v>0.1213640922768305</v>
       </c>
       <c r="H22" s="3" t="s">
@@ -6706,7 +6706,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B23" s="2">
         <v>6</v>
@@ -6721,17 +6721,17 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="F23" s="2">
-        <f>D23-E23</f>
+        <f t="shared" si="0"/>
         <v>7.7100000000000002E-2</v>
       </c>
       <c r="G23" s="2">
-        <f>F23/C23</f>
+        <f t="shared" si="1"/>
         <v>0.12773359840954274</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B24" s="2">
         <v>6</v>
@@ -6746,15 +6746,15 @@
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="F24" s="2">
-        <f>D24-E24</f>
+        <f t="shared" si="0"/>
         <v>8.3199999999999996E-2</v>
       </c>
       <c r="G24" s="2">
-        <f>F24/C24</f>
+        <f t="shared" si="1"/>
         <v>0.12133586116377425</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -6774,11 +6774,11 @@
         <v>9.7999999999999997E-3</v>
       </c>
       <c r="F25" s="2">
-        <f>D25-E25</f>
+        <f t="shared" si="0"/>
         <v>6.5599999999999992E-2</v>
       </c>
       <c r="G25" s="2">
-        <f>F25/C25</f>
+        <f t="shared" si="1"/>
         <v>0.10086100861008609</v>
       </c>
       <c r="H25" s="3" t="s">
@@ -6805,11 +6805,11 @@
         <v>1.24E-2</v>
       </c>
       <c r="F26" s="2">
-        <f>D26-E26</f>
+        <f t="shared" si="0"/>
         <v>7.7700000000000005E-2</v>
       </c>
       <c r="G26" s="2">
-        <f>F26/C26</f>
+        <f t="shared" si="1"/>
         <v>0.14890762744346492</v>
       </c>
       <c r="H26" s="3" t="s">
@@ -6833,11 +6833,11 @@
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="F27" s="2">
-        <f>D27-E27</f>
+        <f t="shared" si="0"/>
         <v>5.8300000000000005E-2</v>
       </c>
       <c r="G27" s="2">
-        <f>F27/C27</f>
+        <f t="shared" si="1"/>
         <v>0.16171983356449376</v>
       </c>
     </row>
@@ -6858,11 +6858,11 @@
         <v>1.34E-2</v>
       </c>
       <c r="F28" s="2">
-        <f>D28-E28</f>
+        <f t="shared" si="0"/>
         <v>8.2799999999999999E-2</v>
       </c>
       <c r="G28" s="2">
-        <f>F28/C28</f>
+        <f t="shared" si="1"/>
         <v>0.14754098360655737</v>
       </c>
     </row>
@@ -6883,11 +6883,11 @@
         <v>1.12E-2</v>
       </c>
       <c r="F29" s="2">
-        <f>D29-E29</f>
+        <f t="shared" si="0"/>
         <v>6.6599999999999993E-2</v>
       </c>
       <c r="G29" s="2">
-        <f>F29/C29</f>
+        <f t="shared" si="1"/>
         <v>0.13107655973233615</v>
       </c>
     </row>
@@ -6908,11 +6908,11 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F30" s="2">
-        <f>D30-E30</f>
+        <f t="shared" si="0"/>
         <v>7.6799999999999993E-2</v>
       </c>
       <c r="G30" s="2">
-        <f>F30/C30</f>
+        <f t="shared" si="1"/>
         <v>0.1292059219380888</v>
       </c>
       <c r="H30" s="3" t="s">
@@ -6936,11 +6936,11 @@
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="F31" s="2">
-        <f>D31-E31</f>
+        <f t="shared" si="0"/>
         <v>6.5500000000000003E-2</v>
       </c>
       <c r="G31" s="2">
-        <f>F31/C31</f>
+        <f t="shared" si="1"/>
         <v>0.11980976769709166</v>
       </c>
       <c r="H31" s="3" t="s">
@@ -6964,11 +6964,11 @@
         <v>1.4200000000000001E-2</v>
       </c>
       <c r="F32" s="2">
-        <f>D32-E32</f>
+        <f t="shared" si="0"/>
         <v>6.8999999999999992E-2</v>
       </c>
       <c r="G32" s="2">
-        <f>F32/C32</f>
+        <f t="shared" si="1"/>
         <v>0.11234125691957017</v>
       </c>
       <c r="H32" s="3" t="s">
@@ -6992,18 +6992,18 @@
         <v>1.6199999999999999E-2</v>
       </c>
       <c r="F33" s="2">
-        <f>D33-E33</f>
+        <f t="shared" si="0"/>
         <v>7.7000000000000013E-2</v>
       </c>
       <c r="G33" s="2">
-        <f>F33/C33</f>
+        <f t="shared" si="1"/>
         <v>0.11213047910295619</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>27</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -7023,11 +7023,11 @@
         <v>1.78E-2</v>
       </c>
       <c r="F34" s="2">
-        <f>D34-E34</f>
+        <f t="shared" ref="F34:F65" si="2">D34-E34</f>
         <v>9.7100000000000006E-2</v>
       </c>
       <c r="G34" s="2">
-        <f>F34/C34</f>
+        <f t="shared" ref="G34:G65" si="3">F34/C34</f>
         <v>0.11905345757724375</v>
       </c>
       <c r="H34" s="3" t="s">
@@ -7054,11 +7054,11 @@
         <v>1.44E-2</v>
       </c>
       <c r="F35" s="2">
-        <f>D35-E35</f>
+        <f t="shared" si="2"/>
         <v>7.9100000000000004E-2</v>
       </c>
       <c r="G35" s="2">
-        <f>F35/C35</f>
+        <f t="shared" si="3"/>
         <v>0.14277978339350181</v>
       </c>
       <c r="H35" s="3" t="s">
@@ -7082,11 +7082,11 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F36" s="2">
-        <f>D36-E36</f>
+        <f t="shared" si="2"/>
         <v>9.4E-2</v>
       </c>
       <c r="G36" s="2">
-        <f>F36/C36</f>
+        <f t="shared" si="3"/>
         <v>0.14154494804999246</v>
       </c>
       <c r="H36" s="3" t="s">
@@ -7095,7 +7095,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B37" s="2">
         <v>6</v>
@@ -7110,11 +7110,11 @@
         <v>1.34E-2</v>
       </c>
       <c r="F37" s="2">
-        <f>D37-E37</f>
+        <f t="shared" si="2"/>
         <v>8.8300000000000003E-2</v>
       </c>
       <c r="G37" s="2">
-        <f>F37/C37</f>
+        <f t="shared" si="3"/>
         <v>0.14770826363332218</v>
       </c>
     </row>
@@ -7135,23 +7135,23 @@
         <v>1.95E-2</v>
       </c>
       <c r="F38" s="2">
-        <f>D38-E38</f>
+        <f t="shared" si="2"/>
         <v>9.7799999999999998E-2</v>
       </c>
       <c r="G38" s="2">
-        <f>F38/C38</f>
+        <f t="shared" si="3"/>
         <v>0.12596599690880989</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>56</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B39" s="2">
         <v>6</v>
@@ -7166,11 +7166,11 @@
         <v>1.1900000000000001E-2</v>
       </c>
       <c r="F39" s="2">
-        <f>D39-E39</f>
+        <f t="shared" si="2"/>
         <v>7.1500000000000008E-2</v>
       </c>
       <c r="G39" s="2">
-        <f>F39/C39</f>
+        <f t="shared" si="3"/>
         <v>0.1359574063510173</v>
       </c>
     </row>
@@ -7191,18 +7191,18 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F40" s="2">
-        <f>D40-E40</f>
+        <f t="shared" si="2"/>
         <v>7.0900000000000005E-2</v>
       </c>
       <c r="G40" s="2">
-        <f>F40/C40</f>
+        <f t="shared" si="3"/>
         <v>0.15850659512631346</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>57</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -7222,11 +7222,11 @@
         <v>1.04E-2</v>
       </c>
       <c r="F41" s="2">
-        <f>D41-E41</f>
+        <f t="shared" si="2"/>
         <v>7.1099999999999997E-2</v>
       </c>
       <c r="G41" s="2">
-        <f>F41/C41</f>
+        <f t="shared" si="3"/>
         <v>0.14778632300976927</v>
       </c>
       <c r="H41" s="3" t="s">
@@ -7250,18 +7250,18 @@
         <v>1.37E-2</v>
       </c>
       <c r="F42" s="2">
-        <f>D42-E42</f>
+        <f t="shared" si="2"/>
         <v>5.7099999999999998E-2</v>
       </c>
       <c r="G42" s="2">
-        <f>F42/C42</f>
+        <f t="shared" si="3"/>
         <v>0.12571554381329811</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -7281,17 +7281,17 @@
         <v>1.12E-2</v>
       </c>
       <c r="F43" s="2">
-        <f>D43-E43</f>
+        <f t="shared" si="2"/>
         <v>7.1899999999999992E-2</v>
       </c>
       <c r="G43" s="2">
-        <f>F43/C43</f>
+        <f t="shared" si="3"/>
         <v>0.12147322182801149</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="2">
         <v>6</v>
@@ -7306,18 +7306,18 @@
         <v>1.6299999999999999E-2</v>
       </c>
       <c r="F44" s="2">
-        <f>D44-E44</f>
+        <f t="shared" si="2"/>
         <v>9.3400000000000011E-2</v>
       </c>
       <c r="G44" s="2">
-        <f>F44/C44</f>
+        <f t="shared" si="3"/>
         <v>0.12352863377860072</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>108</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -7337,18 +7337,18 @@
         <v>1.61E-2</v>
       </c>
       <c r="F45" s="2">
-        <f>D45-E45</f>
+        <f t="shared" si="2"/>
         <v>8.3099999999999993E-2</v>
       </c>
       <c r="G45" s="2">
-        <f>F45/C45</f>
+        <f t="shared" si="3"/>
         <v>0.16720321931589535</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -7368,11 +7368,11 @@
         <v>1.1599999999999999E-2</v>
       </c>
       <c r="F46" s="2">
-        <f>D46-E46</f>
+        <f t="shared" si="2"/>
         <v>8.1199999999999994E-2</v>
       </c>
       <c r="G46" s="2">
-        <f>F46/C46</f>
+        <f t="shared" si="3"/>
         <v>0.16470588235294117</v>
       </c>
     </row>
@@ -7393,11 +7393,11 @@
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="F47" s="2">
-        <f>D47-E47</f>
+        <f t="shared" si="2"/>
         <v>6.6500000000000004E-2</v>
       </c>
       <c r="G47" s="2">
-        <f>F47/C47</f>
+        <f t="shared" si="3"/>
         <v>9.6223411951960644E-2</v>
       </c>
       <c r="H47" s="3" t="s">
@@ -7409,7 +7409,7 @@
     </row>
     <row r="48" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48" s="2">
         <v>6</v>
@@ -7424,11 +7424,11 @@
         <v>1.7299999999999999E-2</v>
       </c>
       <c r="F48" s="2">
-        <f>D48-E48</f>
+        <f t="shared" si="2"/>
         <v>0.10110000000000001</v>
       </c>
       <c r="G48" s="2">
-        <f>F48/C48</f>
+        <f t="shared" si="3"/>
         <v>0.12461481572784421</v>
       </c>
       <c r="H48" s="3" t="s">
@@ -7437,7 +7437,7 @@
     </row>
     <row r="49" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B49" s="2">
         <v>6</v>
@@ -7452,15 +7452,15 @@
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="F49" s="2">
-        <f>D49-E49</f>
+        <f t="shared" si="2"/>
         <v>6.93E-2</v>
       </c>
       <c r="G49" s="2">
-        <f>F49/C49</f>
+        <f t="shared" si="3"/>
         <v>0.14145744029393753</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -7480,11 +7480,11 @@
         <v>1.23E-2</v>
       </c>
       <c r="F50" s="2">
-        <f>D50-E50</f>
+        <f t="shared" si="2"/>
         <v>6.989999999999999E-2</v>
       </c>
       <c r="G50" s="2">
-        <f>F50/C50</f>
+        <f t="shared" si="3"/>
         <v>0.15302101576182134</v>
       </c>
     </row>
@@ -7505,18 +7505,18 @@
         <v>1.6199999999999999E-2</v>
       </c>
       <c r="F51" s="2">
-        <f>D51-E51</f>
+        <f t="shared" si="2"/>
         <v>8.660000000000001E-2</v>
       </c>
       <c r="G51" s="2">
-        <f>F51/C51</f>
+        <f t="shared" si="3"/>
         <v>0.13428438517599628</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>108</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -7536,11 +7536,11 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="F52" s="2">
-        <f>D52-E52</f>
+        <f t="shared" si="2"/>
         <v>6.93E-2</v>
       </c>
       <c r="G52" s="2">
-        <f>F52/C52</f>
+        <f t="shared" si="3"/>
         <v>0.13561643835616438</v>
       </c>
       <c r="H52" s="3" t="s">
@@ -7564,11 +7564,11 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="F53" s="2">
-        <f>D53-E53</f>
+        <f t="shared" si="2"/>
         <v>7.9299999999999995E-2</v>
       </c>
       <c r="G53" s="2">
-        <f>F53/C53</f>
+        <f t="shared" si="3"/>
         <v>0.12904800650935719</v>
       </c>
       <c r="H53" s="3" t="s">
@@ -7595,11 +7595,11 @@
         <v>1.41E-2</v>
       </c>
       <c r="F54" s="2">
-        <f>D54-E54</f>
+        <f t="shared" si="2"/>
         <v>8.1199999999999994E-2</v>
       </c>
       <c r="G54" s="2">
-        <f>F54/C54</f>
+        <f t="shared" si="3"/>
         <v>0.14812112367748995</v>
       </c>
     </row>
@@ -7620,11 +7620,11 @@
         <v>8.6E-3</v>
       </c>
       <c r="F55" s="2">
-        <f>D55-E55</f>
+        <f t="shared" si="2"/>
         <v>5.1900000000000002E-2</v>
       </c>
       <c r="G55" s="2">
-        <f>F55/C55</f>
+        <f t="shared" si="3"/>
         <v>0.15632530120481927</v>
       </c>
     </row>
@@ -7645,11 +7645,11 @@
         <v>1.01E-2</v>
       </c>
       <c r="F56" s="2">
-        <f>D56-E56</f>
+        <f t="shared" si="2"/>
         <v>6.5500000000000003E-2</v>
       </c>
       <c r="G56" s="2">
-        <f>F56/C56</f>
+        <f t="shared" si="3"/>
         <v>0.1159702549575071</v>
       </c>
       <c r="H56" s="3" t="s">
@@ -7658,7 +7658,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B57" s="2">
         <v>6</v>
@@ -7673,11 +7673,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="F57" s="2">
-        <f>D57-E57</f>
+        <f t="shared" si="2"/>
         <v>6.0500000000000005E-2</v>
       </c>
       <c r="G57" s="2">
-        <f>F57/C57</f>
+        <f t="shared" si="3"/>
         <v>0.13462394303515798</v>
       </c>
     </row>
@@ -7698,11 +7698,11 @@
         <v>1.14E-2</v>
       </c>
       <c r="F58" s="2">
-        <f>D58-E58</f>
+        <f t="shared" si="2"/>
         <v>6.9399999999999989E-2</v>
       </c>
       <c r="G58" s="2">
-        <f>F58/C58</f>
+        <f t="shared" si="3"/>
         <v>0.12457368515526833</v>
       </c>
       <c r="H58" s="3" t="s">
@@ -7726,11 +7726,11 @@
         <v>1.1299999999999999E-2</v>
       </c>
       <c r="F59" s="2">
-        <f>D59-E59</f>
+        <f t="shared" si="2"/>
         <v>6.9800000000000001E-2</v>
       </c>
       <c r="G59" s="2">
-        <f>F59/C59</f>
+        <f t="shared" si="3"/>
         <v>0.12890120036934441</v>
       </c>
       <c r="H59" s="3" t="s">
@@ -7754,11 +7754,11 @@
         <v>1.0800000000000001E-2</v>
       </c>
       <c r="F60" s="2">
-        <f>D60-E60</f>
+        <f t="shared" si="2"/>
         <v>8.4099999999999994E-2</v>
       </c>
       <c r="G60" s="2">
-        <f>F60/C60</f>
+        <f t="shared" si="3"/>
         <v>0.15565426614843605</v>
       </c>
       <c r="H60" s="3" t="s">
@@ -7782,17 +7782,17 @@
         <v>1.1599999999999999E-2</v>
       </c>
       <c r="F61" s="2">
-        <f>D61-E61</f>
+        <f t="shared" si="2"/>
         <v>6.4700000000000008E-2</v>
       </c>
       <c r="G61" s="2">
-        <f>F61/C61</f>
+        <f t="shared" si="3"/>
         <v>0.12746256895193064</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B62" s="2">
         <v>6</v>
@@ -7807,11 +7807,11 @@
         <v>7.9000000000000008E-3</v>
       </c>
       <c r="F62" s="2">
-        <f>D62-E62</f>
+        <f t="shared" si="2"/>
         <v>4.99E-2</v>
       </c>
       <c r="G62" s="2">
-        <f>F62/C62</f>
+        <f t="shared" si="3"/>
         <v>0.14612005856515373</v>
       </c>
       <c r="H62" s="3" t="s">
@@ -7835,11 +7835,11 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="F63" s="2">
-        <f>D63-E63</f>
+        <f t="shared" si="2"/>
         <v>6.3899999999999998E-2</v>
       </c>
       <c r="G63" s="2">
-        <f>F63/C63</f>
+        <f t="shared" si="3"/>
         <v>0.14716720405343162</v>
       </c>
     </row>
@@ -7860,11 +7860,11 @@
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="F64" s="2">
-        <f>D64-E64</f>
+        <f t="shared" si="2"/>
         <v>5.2400000000000002E-2</v>
       </c>
       <c r="G64" s="2">
-        <f>F64/C64</f>
+        <f t="shared" si="3"/>
         <v>0.1529034140647797</v>
       </c>
       <c r="H64" s="3" t="s">
@@ -7888,11 +7888,11 @@
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="F65" s="2">
-        <f>D65-E65</f>
+        <f t="shared" si="2"/>
         <v>5.8099999999999999E-2</v>
       </c>
       <c r="G65" s="2">
-        <f>F65/C65</f>
+        <f t="shared" si="3"/>
         <v>0.13384012900253398</v>
       </c>
       <c r="H65" s="3" t="s">
@@ -7916,11 +7916,11 @@
         <v>6.1000000000000004E-3</v>
       </c>
       <c r="F66" s="2">
-        <f>D66-E66</f>
+        <f t="shared" ref="F66:F97" si="4">D66-E66</f>
         <v>3.9599999999999996E-2</v>
       </c>
       <c r="G66" s="2">
-        <f>F66/C66</f>
+        <f t="shared" ref="G66:G97" si="5">F66/C66</f>
         <v>0.15695600475624255</v>
       </c>
       <c r="H66" s="3" t="s">
@@ -7944,11 +7944,11 @@
         <v>7.6E-3</v>
       </c>
       <c r="F67" s="2">
-        <f>D67-E67</f>
+        <f t="shared" si="4"/>
         <v>4.8799999999999996E-2</v>
       </c>
       <c r="G67" s="2">
-        <f>F67/C67</f>
+        <f t="shared" si="5"/>
         <v>0.1096629213483146</v>
       </c>
       <c r="H67" s="3" t="s">
@@ -7972,11 +7972,11 @@
         <v>8.3999999999999995E-3</v>
       </c>
       <c r="F68" s="2">
-        <f>D68-E68</f>
+        <f t="shared" si="4"/>
         <v>5.0300000000000004E-2</v>
       </c>
       <c r="G68" s="2">
-        <f>F68/C68</f>
+        <f t="shared" si="5"/>
         <v>0.14707602339181286</v>
       </c>
       <c r="H68" s="3" t="s">
@@ -8000,11 +8000,11 @@
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="F69" s="2">
-        <f>D69-E69</f>
+        <f t="shared" si="4"/>
         <v>5.9800000000000006E-2</v>
       </c>
       <c r="G69" s="2">
-        <f>F69/C69</f>
+        <f t="shared" si="5"/>
         <v>0.13842592592592595</v>
       </c>
       <c r="H69" s="3" t="s">
@@ -8013,7 +8013,7 @@
     </row>
     <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B70" s="2">
         <v>5</v>
@@ -8028,15 +8028,15 @@
         <v>8.6999999999999994E-3</v>
       </c>
       <c r="F70" s="2">
-        <f>D70-E70</f>
+        <f t="shared" si="4"/>
         <v>6.4100000000000004E-2</v>
       </c>
       <c r="G70" s="2">
-        <f>F70/C70</f>
+        <f t="shared" si="5"/>
         <v>0.14598041448417218</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>28</v>
@@ -8059,11 +8059,11 @@
         <v>1.26E-2</v>
       </c>
       <c r="F71" s="2">
-        <f>D71-E71</f>
+        <f t="shared" si="4"/>
         <v>6.7400000000000002E-2</v>
       </c>
       <c r="G71" s="2">
-        <f>F71/C71</f>
+        <f t="shared" si="5"/>
         <v>0.11803852889667252</v>
       </c>
       <c r="H71" s="3" t="s">
@@ -8087,17 +8087,17 @@
         <v>1.24E-2</v>
       </c>
       <c r="F72" s="2">
-        <f>D72-E72</f>
+        <f t="shared" si="4"/>
         <v>6.5500000000000003E-2</v>
       </c>
       <c r="G72" s="2">
-        <f>F72/C72</f>
+        <f t="shared" si="5"/>
         <v>0.13798188329471245</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B73" s="2">
         <v>6</v>
@@ -8112,11 +8112,11 @@
         <v>7.6E-3</v>
       </c>
       <c r="F73" s="2">
-        <f>D73-E73</f>
+        <f t="shared" si="4"/>
         <v>4.6799999999999994E-2</v>
       </c>
       <c r="G73" s="2">
-        <f>F73/C73</f>
+        <f t="shared" si="5"/>
         <v>0.15249266862170086</v>
       </c>
     </row>
@@ -8137,11 +8137,11 @@
         <v>1.1900000000000001E-2</v>
       </c>
       <c r="F74" s="2">
-        <f>D74-E74</f>
+        <f t="shared" si="4"/>
         <v>6.720000000000001E-2</v>
       </c>
       <c r="G74" s="2">
-        <f>F74/C74</f>
+        <f t="shared" si="5"/>
         <v>0.13112195121951223</v>
       </c>
     </row>
@@ -8162,11 +8162,11 @@
         <v>8.6999999999999994E-3</v>
       </c>
       <c r="F75" s="2">
-        <f>D75-E75</f>
+        <f t="shared" si="4"/>
         <v>5.7900000000000007E-2</v>
       </c>
       <c r="G75" s="2">
-        <f>F75/C75</f>
+        <f t="shared" si="5"/>
         <v>0.14275147928994084</v>
       </c>
       <c r="H75" s="3" t="s">
@@ -8190,15 +8190,15 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="F76" s="2">
-        <f>D76-E76</f>
+        <f t="shared" si="4"/>
         <v>6.8599999999999994E-2</v>
       </c>
       <c r="G76" s="2">
-        <f>F76/C76</f>
+        <f t="shared" si="5"/>
         <v>0.13289422704378148</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -8218,11 +8218,11 @@
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="F77" s="2">
-        <f>D77-E77</f>
+        <f t="shared" si="4"/>
         <v>4.5499999999999999E-2</v>
       </c>
       <c r="G77" s="2">
-        <f>F77/C77</f>
+        <f t="shared" si="5"/>
         <v>0.15668044077134985</v>
       </c>
     </row>
@@ -8243,11 +8243,11 @@
         <v>1.15E-2</v>
       </c>
       <c r="F78" s="2">
-        <f>D78-E78</f>
+        <f t="shared" si="4"/>
         <v>6.6200000000000009E-2</v>
       </c>
       <c r="G78" s="2">
-        <f>F78/C78</f>
+        <f t="shared" si="5"/>
         <v>0.14088103851883382</v>
       </c>
       <c r="H78" s="3" t="s">
@@ -8271,11 +8271,11 @@
         <v>1.0500000000000001E-2</v>
       </c>
       <c r="F79" s="2">
-        <f>D79-E79</f>
+        <f t="shared" si="4"/>
         <v>6.9100000000000009E-2</v>
       </c>
       <c r="G79" s="2">
-        <f>F79/C79</f>
+        <f t="shared" si="5"/>
         <v>0.14206414473684212</v>
       </c>
       <c r="H79" s="3" t="s">
@@ -8299,11 +8299,11 @@
         <v>1.15E-2</v>
       </c>
       <c r="F80" s="2">
-        <f>D80-E80</f>
+        <f t="shared" si="4"/>
         <v>6.770000000000001E-2</v>
       </c>
       <c r="G80" s="2">
-        <f>F80/C80</f>
+        <f t="shared" si="5"/>
         <v>0.15467214987434319</v>
       </c>
       <c r="H80" s="3" t="s">
@@ -8330,11 +8330,11 @@
         <v>7.4000000000000003E-3</v>
       </c>
       <c r="F81" s="2">
-        <f>D81-E81</f>
+        <f t="shared" si="4"/>
         <v>4.6799999999999994E-2</v>
       </c>
       <c r="G81" s="2">
-        <f>F81/C81</f>
+        <f t="shared" si="5"/>
         <v>0.17092768444119794</v>
       </c>
     </row>
@@ -8355,11 +8355,11 @@
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="F82" s="2">
-        <f>D82-E82</f>
+        <f t="shared" si="4"/>
         <v>4.6699999999999998E-2</v>
       </c>
       <c r="G82" s="2">
-        <f>F82/C82</f>
+        <f t="shared" si="5"/>
         <v>0.14616588419405321</v>
       </c>
       <c r="H82" s="3" t="s">
@@ -8383,18 +8383,18 @@
         <v>1.37E-2</v>
       </c>
       <c r="F83" s="2">
-        <f>D83-E83</f>
+        <f t="shared" si="4"/>
         <v>6.7099999999999993E-2</v>
       </c>
       <c r="G83" s="2">
-        <f>F83/C83</f>
+        <f t="shared" si="5"/>
         <v>0.1418304798139928</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>86</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -8414,11 +8414,11 @@
         <v>7.9000000000000008E-3</v>
       </c>
       <c r="F84" s="2">
-        <f>D84-E84</f>
+        <f t="shared" si="4"/>
         <v>4.8799999999999996E-2</v>
       </c>
       <c r="G84" s="2">
-        <f>F84/C84</f>
+        <f t="shared" si="5"/>
         <v>0.1515527950310559</v>
       </c>
       <c r="H84" s="3" t="s">
@@ -8442,11 +8442,11 @@
         <v>7.4000000000000003E-3</v>
       </c>
       <c r="F85" s="2">
-        <f>D85-E85</f>
+        <f t="shared" si="4"/>
         <v>4.7500000000000001E-2</v>
       </c>
       <c r="G85" s="2">
-        <f>F85/C85</f>
+        <f t="shared" si="5"/>
         <v>0.1736111111111111</v>
       </c>
       <c r="H85" s="3" t="s">
@@ -8470,11 +8470,11 @@
         <v>8.6999999999999994E-3</v>
       </c>
       <c r="F86" s="2">
-        <f>D86-E86</f>
+        <f t="shared" si="4"/>
         <v>6.7199999999999996E-2</v>
       </c>
       <c r="G86" s="2">
-        <f>F86/C86</f>
+        <f t="shared" si="5"/>
         <v>0.16880180859080632</v>
       </c>
       <c r="H86" s="3" t="s">
@@ -8498,11 +8498,11 @@
         <v>1.41E-2</v>
       </c>
       <c r="F87" s="2">
-        <f>D87-E87</f>
+        <f t="shared" si="4"/>
         <v>7.5600000000000001E-2</v>
       </c>
       <c r="G87" s="2">
-        <f>F87/C87</f>
+        <f t="shared" si="5"/>
         <v>0.14261460101867571</v>
       </c>
     </row>
@@ -8523,11 +8523,11 @@
         <v>1.01E-2</v>
       </c>
       <c r="F88" s="2">
-        <f>D88-E88</f>
+        <f t="shared" si="4"/>
         <v>6.5799999999999997E-2</v>
       </c>
       <c r="G88" s="2">
-        <f>F88/C88</f>
+        <f t="shared" si="5"/>
         <v>0.12871674491392801</v>
       </c>
       <c r="H88" s="3" t="s">
@@ -8551,18 +8551,18 @@
         <v>9.9000000000000008E-3</v>
       </c>
       <c r="F89" s="2">
-        <f>D89-E89</f>
+        <f t="shared" si="4"/>
         <v>6.9999999999999993E-2</v>
       </c>
       <c r="G89" s="2">
-        <f>F89/C89</f>
+        <f t="shared" si="5"/>
         <v>0.11484823625922885</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>60</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -8582,11 +8582,11 @@
         <v>1.01E-2</v>
       </c>
       <c r="F90" s="2">
-        <f>D90-E90</f>
+        <f t="shared" si="4"/>
         <v>5.9800000000000006E-2</v>
       </c>
       <c r="G90" s="2">
-        <f>F90/C90</f>
+        <f t="shared" si="5"/>
         <v>0.16049382716049385</v>
       </c>
       <c r="H90" s="3" t="s">
@@ -8610,11 +8610,11 @@
         <v>9.1000000000000004E-3</v>
       </c>
       <c r="F91" s="2">
-        <f>D91-E91</f>
+        <f t="shared" si="4"/>
         <v>5.7800000000000004E-2</v>
       </c>
       <c r="G91" s="2">
-        <f>F91/C91</f>
+        <f t="shared" si="5"/>
         <v>0.15874759681406209</v>
       </c>
       <c r="H91" s="3" t="s">
@@ -8638,11 +8638,11 @@
         <v>8.8999999999999999E-3</v>
       </c>
       <c r="F92" s="2">
-        <f>D92-E92</f>
+        <f t="shared" si="4"/>
         <v>5.8699999999999995E-2</v>
       </c>
       <c r="G92" s="2">
-        <f>F92/C92</f>
+        <f t="shared" si="5"/>
         <v>0.14141170802216332</v>
       </c>
       <c r="H92" s="3" t="s">
@@ -8666,11 +8666,11 @@
         <v>7.4000000000000003E-3</v>
       </c>
       <c r="F93" s="2">
-        <f>D93-E93</f>
+        <f t="shared" si="4"/>
         <v>4.9500000000000002E-2</v>
       </c>
       <c r="G93" s="2">
-        <f>F93/C93</f>
+        <f t="shared" si="5"/>
         <v>0.16108037748128864</v>
       </c>
       <c r="H93" s="3" t="s">
@@ -8694,11 +8694,11 @@
         <v>8.6E-3</v>
       </c>
       <c r="F94" s="2">
-        <f>D94-E94</f>
+        <f t="shared" si="4"/>
         <v>4.6600000000000003E-2</v>
       </c>
       <c r="G94" s="2">
-        <f>F94/C94</f>
+        <f t="shared" si="5"/>
         <v>0.17388059701492536</v>
       </c>
     </row>
@@ -8719,18 +8719,18 @@
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="F95" s="2">
-        <f>D95-E95</f>
+        <f t="shared" si="4"/>
         <v>7.4399999999999994E-2</v>
       </c>
       <c r="G95" s="2">
-        <f>F95/C95</f>
+        <f t="shared" si="5"/>
         <v>0.17854571634269256</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>56</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -8750,11 +8750,11 @@
         <v>1.54E-2</v>
       </c>
       <c r="F96" s="2">
-        <f>D96-E96</f>
+        <f t="shared" si="4"/>
         <v>7.8200000000000006E-2</v>
       </c>
       <c r="G96" s="2">
-        <f>F96/C96</f>
+        <f t="shared" si="5"/>
         <v>0.15887850467289719</v>
       </c>
       <c r="H96" s="3" t="s">
@@ -8778,11 +8778,11 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="F97" s="2">
-        <f>D97-E97</f>
+        <f t="shared" si="4"/>
         <v>4.0899999999999999E-2</v>
       </c>
       <c r="G97" s="2">
-        <f>F97/C97</f>
+        <f t="shared" si="5"/>
         <v>0.12534477474716518</v>
       </c>
       <c r="H97" s="3" t="s">
@@ -8809,11 +8809,11 @@
         <v>1.38E-2</v>
       </c>
       <c r="F98" s="2">
-        <f>D98-E98</f>
+        <f t="shared" ref="F98:F108" si="6">D98-E98</f>
         <v>7.3099999999999998E-2</v>
       </c>
       <c r="G98" s="2">
-        <f>F98/C98</f>
+        <f t="shared" ref="G98:G108" si="7">F98/C98</f>
         <v>0.15583031336602002</v>
       </c>
       <c r="H98" s="3" t="s">
@@ -8837,11 +8837,11 @@
         <v>8.3999999999999995E-3</v>
       </c>
       <c r="F99" s="2">
-        <f>D99-E99</f>
+        <f t="shared" si="6"/>
         <v>5.7600000000000005E-2</v>
       </c>
       <c r="G99" s="2">
-        <f>F99/C99</f>
+        <f t="shared" si="7"/>
         <v>0.11180124223602486</v>
       </c>
       <c r="H99" s="3" t="s">
@@ -8868,11 +8868,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="F100" s="2">
-        <f>D100-E100</f>
+        <f t="shared" si="6"/>
         <v>5.8699999999999995E-2</v>
       </c>
       <c r="G100" s="2">
-        <f>F100/C100</f>
+        <f t="shared" si="7"/>
         <v>0.15990193407790793</v>
       </c>
       <c r="H100" s="3" t="s">
@@ -8896,11 +8896,11 @@
         <v>0.01</v>
       </c>
       <c r="F101" s="2">
-        <f>D101-E101</f>
+        <f t="shared" si="6"/>
         <v>6.4899999999999999E-2</v>
       </c>
       <c r="G101" s="2">
-        <f>F101/C101</f>
+        <f t="shared" si="7"/>
         <v>0.15216881594372803</v>
       </c>
       <c r="H101" s="3" t="s">
@@ -8909,7 +8909,7 @@
     </row>
     <row r="102" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B102" s="2">
         <v>6</v>
@@ -8924,15 +8924,15 @@
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="F102" s="2">
-        <f>D102-E102</f>
+        <f t="shared" si="6"/>
         <v>7.4700000000000003E-2</v>
       </c>
       <c r="G102" s="2">
-        <f>F102/C102</f>
+        <f t="shared" si="7"/>
         <v>0.15673520772135963</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
@@ -8952,11 +8952,11 @@
         <v>9.7999999999999997E-3</v>
       </c>
       <c r="F103" s="2">
-        <f>D103-E103</f>
+        <f t="shared" si="6"/>
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="G103" s="2">
-        <f>F103/C103</f>
+        <f t="shared" si="7"/>
         <v>0.15579994763026969</v>
       </c>
     </row>
@@ -8977,18 +8977,18 @@
         <v>1.3899999999999999E-2</v>
       </c>
       <c r="F104" s="2">
-        <f>D104-E104</f>
+        <f t="shared" si="6"/>
         <v>6.8900000000000003E-2</v>
       </c>
       <c r="G104" s="2">
-        <f>F104/C104</f>
+        <f t="shared" si="7"/>
         <v>0.15535512965050732</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>86</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -9008,11 +9008,11 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="F105" s="2">
-        <f>D105-E105</f>
+        <f t="shared" si="6"/>
         <v>5.45E-2</v>
       </c>
       <c r="G105" s="2">
-        <f>F105/C105</f>
+        <f t="shared" si="7"/>
         <v>0.16836577077540935</v>
       </c>
       <c r="H105" s="3" t="s">
@@ -9036,11 +9036,11 @@
         <v>1.4200000000000001E-2</v>
       </c>
       <c r="F106" s="2">
-        <f>D106-E106</f>
+        <f t="shared" si="6"/>
         <v>8.1599999999999992E-2</v>
       </c>
       <c r="G106" s="2">
-        <f>F106/C106</f>
+        <f t="shared" si="7"/>
         <v>0.16238805970149253</v>
       </c>
     </row>
@@ -9061,11 +9061,11 @@
         <v>8.8999999999999999E-3</v>
       </c>
       <c r="F107" s="2">
-        <f>D107-E107</f>
+        <f t="shared" si="6"/>
         <v>5.7700000000000008E-2</v>
       </c>
       <c r="G107" s="2">
-        <f>F107/C107</f>
+        <f t="shared" si="7"/>
         <v>0.16822157434402332</v>
       </c>
     </row>
@@ -9086,11 +9086,11 @@
         <v>8.6999999999999994E-3</v>
       </c>
       <c r="F108" s="2">
-        <f>D108-E108</f>
+        <f t="shared" si="6"/>
         <v>4.9700000000000001E-2</v>
       </c>
       <c r="G108" s="2">
-        <f>F108/C108</f>
+        <f t="shared" si="7"/>
         <v>0.20211468076453842</v>
       </c>
       <c r="H108" s="3" t="s">

</xml_diff>